<commit_message>
Update simple earthquake data
</commit_message>
<xml_diff>
--- a/pynewmarkdisp/earthquake_data_simple.xlsx
+++ b/pynewmarkdisp/earthquake_data_simple.xlsx
@@ -1,53 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EAMA\My Drive\Dev\GitHub\data4testing\pynewmarkdisp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD8FB12-E92C-4DAE-9FE2-8739A1B30B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{198F23FD-65C0-4AB9-8100-5DF83FCFB5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-2850" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="earthquake_data_simple" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Acceleration</t>
+    <t>Time</t>
   </si>
   <si>
-    <t>Time</t>
+    <t>Acceleration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,16 +40,316 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -72,15 +357,204 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -391,1241 +865,1400 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B153"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B173"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:I1048576"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>3.7999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>-3.0000000000000001E-3</v>
+        <v>2.59541984732825E-3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>7.0999999999999994E-2</v>
+        <v>2.8137310073157E-2</v>
       </c>
       <c r="B3">
-        <v>1.0999999999999999E-2</v>
+        <v>8.09160305343503E-3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>0.13600000000000001</v>
+        <v>5.6274620146314E-2</v>
       </c>
       <c r="B4">
-        <v>-0.02</v>
+        <v>1.6335877862595299E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>0.19600000000000001</v>
+        <v>7.87844682048396E-2</v>
       </c>
       <c r="B5">
-        <v>-0.04</v>
+        <v>1.0839694656488499E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>0.22800000000000001</v>
+        <v>0.10129431626336501</v>
       </c>
       <c r="B6">
-        <v>-2.9000000000000001E-2</v>
+        <v>-1.52671755725197E-4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>0.28299999999999997</v>
+        <v>0.112549240292628</v>
       </c>
       <c r="B7">
-        <v>-4.2999999999999997E-2</v>
+        <v>-1.1145038167938799E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>0.34200000000000003</v>
+        <v>0.146314012380416</v>
       </c>
       <c r="B8">
-        <v>-4.5999999999999999E-2</v>
+        <v>-3.31297709923664E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>0.40799999999999997</v>
+        <v>0.18570624648283601</v>
       </c>
       <c r="B9">
-        <v>-5.5E-2</v>
+        <v>-2.2137404580152599E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>0.435</v>
+        <v>0.225098480585256</v>
       </c>
       <c r="B10">
-        <v>-4.5999999999999999E-2</v>
+        <v>-1.9389312977099199E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>0.47299999999999998</v>
+        <v>0.25323579065841201</v>
       </c>
       <c r="B11">
-        <v>5.0000000000000001E-3</v>
+        <v>-2.76335877862595E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>0.5</v>
+        <v>0.28137310073156901</v>
       </c>
       <c r="B12">
-        <v>1.6E-2</v>
+        <v>-4.1374045801526697E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>0.53300000000000003</v>
+        <v>0.34890264490714601</v>
       </c>
       <c r="B13">
-        <v>-1.7999999999999999E-2</v>
+        <v>-4.1374045801526697E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>0.54900000000000004</v>
+        <v>0.37703995498030302</v>
       </c>
       <c r="B14">
-        <v>-4.5999999999999999E-2</v>
+        <v>-4.6870229007633601E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>0.58199999999999996</v>
+        <v>0.40517726505346002</v>
       </c>
       <c r="B15">
-        <v>-2.7E-2</v>
+        <v>-5.5114503816793899E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>0.59799999999999998</v>
+        <v>0.416432189082723</v>
       </c>
       <c r="B16">
-        <v>1.0999999999999999E-2</v>
+        <v>-5.2366412213740499E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>0.63600000000000001</v>
+        <v>0.450196961170512</v>
       </c>
       <c r="B17">
-        <v>-1E-3</v>
+        <v>-2.2137404580152599E-2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>0.66800000000000004</v>
+        <v>0.46145188519977398</v>
       </c>
       <c r="B18">
-        <v>-7.0000000000000001E-3</v>
+        <v>-2.9007633587786398E-3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>0.68500000000000005</v>
+        <v>0.50084411930219397</v>
       </c>
       <c r="B19">
-        <v>0.03</v>
+        <v>2.4580152671755701E-2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>0.71199999999999997</v>
+        <v>0.517726505346088</v>
       </c>
       <c r="B20">
-        <v>6.8000000000000005E-2</v>
+        <v>5.3435114503816898E-3</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>0.71699999999999997</v>
+        <v>0.56274620146314003</v>
       </c>
       <c r="B21">
-        <v>8.7999999999999995E-2</v>
+        <v>-3.5877862595419897E-2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>0.73399999999999999</v>
+        <v>0.57962858750703405</v>
       </c>
       <c r="B22">
-        <v>4.8000000000000001E-2</v>
+        <v>-1.1145038167938799E-2</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>0.755</v>
+        <v>0.60776589758019095</v>
       </c>
       <c r="B23">
-        <v>2.1999999999999999E-2</v>
+        <v>2.18320610687022E-2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>0.78300000000000003</v>
+        <v>0.65841305571187303</v>
       </c>
       <c r="B24">
-        <v>7.0000000000000001E-3</v>
+        <v>-5.6488549618320897E-3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>0.81</v>
+        <v>0.66966797974113601</v>
       </c>
       <c r="B25">
-        <v>3.3000000000000002E-2</v>
+        <v>5.3435114503816898E-3</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>0.85299999999999998</v>
+        <v>0.67529544175576794</v>
       </c>
       <c r="B26">
-        <v>7.0000000000000007E-2</v>
+        <v>2.7328244274809101E-2</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>0.88600000000000001</v>
+        <v>0.68092290377039899</v>
       </c>
       <c r="B27">
-        <v>0.05</v>
+        <v>4.9312977099236599E-2</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>0.91300000000000003</v>
+        <v>0.69217782779966197</v>
       </c>
       <c r="B28">
-        <v>3.5999999999999997E-2</v>
+        <v>7.1297709923663993E-2</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>0.95699999999999996</v>
+        <v>0.70343275182892495</v>
       </c>
       <c r="B29">
-        <v>3.9E-2</v>
+        <v>9.6030534351145003E-2</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>0.97299999999999998</v>
+        <v>0.72031513787281898</v>
       </c>
       <c r="B30">
-        <v>-1.2999999999999999E-2</v>
+        <v>7.4045801526717497E-2</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>0.995</v>
+        <v>0.74845244794597598</v>
       </c>
       <c r="B31">
-        <v>-6.4000000000000001E-2</v>
+        <v>3.2824427480915901E-2</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>1.0109999999999999</v>
+        <v>0.77096229600450095</v>
       </c>
       <c r="B32">
-        <v>-7.5999999999999998E-2</v>
+        <v>5.3435114503816898E-3</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>1.0329999999999999</v>
+        <v>0.79909960607765795</v>
       </c>
       <c r="B33">
-        <v>-4.1000000000000002E-2</v>
+        <v>2.7328244274809101E-2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>1.06</v>
+        <v>0.83849184018007805</v>
       </c>
       <c r="B34">
-        <v>-1.2999999999999999E-2</v>
+        <v>6.3053435114503703E-2</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>1.087</v>
+        <v>0.85537422622397197</v>
       </c>
       <c r="B35">
-        <v>-3.5999999999999997E-2</v>
+        <v>7.6793893129770904E-2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>1.103</v>
+        <v>0.91727630838491803</v>
       </c>
       <c r="B36">
-        <v>-5.6000000000000001E-2</v>
+        <v>3.2824427480915901E-2</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>1.1299999999999999</v>
+        <v>0.95666854248733801</v>
       </c>
       <c r="B37">
-        <v>-0.09</v>
+        <v>4.9312977099236599E-2</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>1.141</v>
+        <v>0.9679234665166</v>
       </c>
       <c r="B38">
-        <v>-0.107</v>
+        <v>1.3587786259541899E-2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>1.1850000000000001</v>
+        <v>0.99043331457512596</v>
       </c>
       <c r="B39">
-        <v>-0.09</v>
+        <v>-3.0381679389313E-2</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>1.212</v>
+        <v>1.01294316263365</v>
       </c>
       <c r="B40">
-        <v>-0.09</v>
+        <v>-6.8854961832060996E-2</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>1.25</v>
+        <v>1.03545301069217</v>
       </c>
       <c r="B41">
-        <v>-9.9000000000000005E-2</v>
+        <v>-4.9618320610687001E-2</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>1.2829999999999999</v>
+        <v>1.0410804727067999</v>
       </c>
       <c r="B42">
-        <v>-6.8000000000000005E-2</v>
+        <v>-3.0381679389313E-2</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>1.31</v>
+        <v>1.06921778277996</v>
       </c>
       <c r="B43">
-        <v>-0.05</v>
+        <v>1.0839694656488499E-2</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>1.3420000000000001</v>
+        <v>1.1029825548677501</v>
       </c>
       <c r="B44">
-        <v>-6.2E-2</v>
+        <v>-3.5877862595419897E-2</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>1.397</v>
+        <v>1.11423747889701</v>
       </c>
       <c r="B45">
-        <v>-3.1E-2</v>
+        <v>-5.7862595419847201E-2</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>1.446</v>
+        <v>1.1254924029262701</v>
       </c>
       <c r="B46">
-        <v>-2.1999999999999999E-2</v>
+        <v>-7.16030534351145E-2</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>1.4730000000000001</v>
+        <v>1.15362971299943</v>
       </c>
       <c r="B47">
-        <v>3.2000000000000001E-2</v>
+        <v>-0.10458015267175499</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>1.5049999999999999</v>
+        <v>1.1817670230725901</v>
       </c>
       <c r="B48">
-        <v>7.8E-2</v>
+        <v>-8.8091603053435094E-2</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>1.5329999999999999</v>
+        <v>1.2211592571750101</v>
       </c>
       <c r="B49">
-        <v>3.7999999999999999E-2</v>
+        <v>-6.8854961832060996E-2</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>1.5429999999999999</v>
+        <v>1.24929656724817</v>
       </c>
       <c r="B50">
-        <v>-5.0000000000000001E-3</v>
+        <v>-9.0839694656488501E-2</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>1.571</v>
+        <v>1.26617895329206</v>
       </c>
       <c r="B51">
-        <v>-3.5999999999999997E-2</v>
+        <v>-9.9083969465648902E-2</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>1.62</v>
+        <v>1.2886888013505899</v>
       </c>
       <c r="B52">
-        <v>-7.6999999999999999E-2</v>
+        <v>-7.16030534351145E-2</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>1.63</v>
+        <v>1.3111986494091099</v>
       </c>
       <c r="B53">
-        <v>-0.111</v>
+        <v>-3.5877862595419897E-2</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>1.679</v>
+        <v>1.3562183455261601</v>
       </c>
       <c r="B54">
-        <v>-0.111</v>
+        <v>-6.0610687022900699E-2</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>1.734</v>
+        <v>1.3899831176139501</v>
       </c>
       <c r="B55">
-        <v>-0.12</v>
+        <v>-4.1374045801526697E-2</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>1.7769999999999999</v>
+        <v>1.4124929656724801</v>
       </c>
       <c r="B56">
-        <v>-0.123</v>
+        <v>-2.48854961832061E-2</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>1.7929999999999999</v>
+        <v>1.45751266178953</v>
       </c>
       <c r="B57">
-        <v>-0.111</v>
+        <v>-2.76335877862595E-2</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>1.821</v>
+        <v>1.4856499718626801</v>
       </c>
       <c r="B58">
-        <v>-0.123</v>
+        <v>5.3435114503816898E-3</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>1.8640000000000001</v>
+        <v>1.5250422059651001</v>
       </c>
       <c r="B59">
-        <v>-0.123</v>
+        <v>7.6793893129770904E-2</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>1.9079999999999999</v>
+        <v>1.57006190208216</v>
       </c>
       <c r="B60">
-        <v>-0.11700000000000001</v>
+        <v>2.59541984732825E-3</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>1.94</v>
+        <v>1.59257175014068</v>
       </c>
       <c r="B61">
-        <v>-0.123</v>
+        <v>-4.4122137404580097E-2</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>1.9570000000000001</v>
+        <v>1.6769836803601501</v>
       </c>
       <c r="B62">
-        <v>-0.111</v>
+        <v>-0.10458015267175499</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>1.9730000000000001</v>
+        <v>1.78390545863815</v>
       </c>
       <c r="B63">
-        <v>-6.9000000000000006E-2</v>
+        <v>-0.118320610687022</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>1.984</v>
+        <v>1.82329769274057</v>
       </c>
       <c r="B64">
-        <v>-1.7000000000000001E-2</v>
+        <v>-9.6335877862595301E-2</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>2.016</v>
+        <v>1.87394485087225</v>
       </c>
       <c r="B65">
-        <v>3.1E-2</v>
+        <v>-0.12106870229007601</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>2.0329999999999999</v>
+        <v>1.9245920090039299</v>
       </c>
       <c r="B66">
-        <v>8.5999999999999993E-2</v>
+        <v>-0.107328244274809</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>2.0430000000000001</v>
+        <v>1.97523916713562</v>
       </c>
       <c r="B67">
-        <v>0.11700000000000001</v>
+        <v>-0.123816793893129</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>2.0649999999999999</v>
+        <v>2.00900393922341</v>
       </c>
       <c r="B68">
-        <v>0.14299999999999999</v>
+        <v>-5.2366412213740499E-2</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>2.0819999999999999</v>
+        <v>2.0371412492965599</v>
       </c>
       <c r="B69">
-        <v>0.19400000000000001</v>
+        <v>1.6335877862595299E-2</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>2.1030000000000002</v>
+        <v>2.0596510973550899</v>
       </c>
       <c r="B70">
-        <v>0.23100000000000001</v>
+        <v>4.3816793893129702E-2</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>2.12</v>
+        <v>2.0877884074282398</v>
       </c>
       <c r="B71">
-        <v>0.28799999999999998</v>
+        <v>0.120763358778625</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>2.141</v>
+        <v>2.1102982554867702</v>
       </c>
       <c r="B72">
-        <v>0.34</v>
+        <v>0.19221374045801501</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>2.1469999999999998</v>
+        <v>2.1328081035453001</v>
       </c>
       <c r="B73">
-        <v>0.40600000000000003</v>
+        <v>0.225190839694656</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>2.1629999999999998</v>
+        <v>2.1496904895891902</v>
       </c>
       <c r="B74">
-        <v>0.44</v>
+        <v>0.26641221374045798</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>2.19</v>
+        <v>2.1722003376477201</v>
       </c>
       <c r="B75">
-        <v>0.48299999999999998</v>
+        <v>0.32412213740458001</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>2.234</v>
+        <v>2.18345526167698</v>
       </c>
       <c r="B76">
-        <v>0.41699999999999998</v>
+        <v>0.36259541984732802</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>2.25</v>
+        <v>2.20033764772087</v>
       </c>
       <c r="B77">
-        <v>0.371</v>
+        <v>0.40931297709923598</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>2.266</v>
+        <v>2.2341024198086599</v>
       </c>
       <c r="B78">
-        <v>0.27700000000000002</v>
+        <v>0.46977099236641201</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>2.2770000000000001</v>
+        <v>2.2734946539110799</v>
       </c>
       <c r="B79">
-        <v>0.19700000000000001</v>
+        <v>0.40931297709923598</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>2.3039999999999998</v>
+        <v>2.2734946539110799</v>
       </c>
       <c r="B80">
-        <v>2E-3</v>
+        <v>0.37358778625954098</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>2.3370000000000002</v>
+        <v>2.2960045019696098</v>
       </c>
       <c r="B81">
-        <v>-0.12</v>
+        <v>0.27465648854961799</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>2.3639999999999999</v>
+        <v>2.30163196398424</v>
       </c>
       <c r="B82">
-        <v>-0.28000000000000003</v>
+        <v>0.19221374045801501</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>2.4079999999999999</v>
+        <v>2.3128868880134998</v>
       </c>
       <c r="B83">
-        <v>-0.40600000000000003</v>
+        <v>6.85496183206106E-2</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>2.4510000000000001</v>
+        <v>2.3353967360720298</v>
       </c>
       <c r="B84">
-        <v>-0.35199999999999998</v>
+        <v>-5.6488549618320897E-3</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>2.4729999999999999</v>
+        <v>2.3691615081598201</v>
       </c>
       <c r="B85">
-        <v>-0.27200000000000002</v>
+        <v>-0.13480916030534301</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>2.4889999999999999</v>
+        <v>2.3916713562183398</v>
       </c>
       <c r="B86">
-        <v>-0.155</v>
+        <v>-0.23374045801526699</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>2.4950000000000001</v>
+        <v>2.39729881823297</v>
       </c>
       <c r="B87">
-        <v>-6.0999999999999999E-2</v>
+        <v>-0.28320610687022801</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>2.5</v>
+        <v>2.4029262802476001</v>
       </c>
       <c r="B88">
-        <v>1.6E-2</v>
+        <v>-0.349160305343511</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>2.516</v>
+        <v>2.4310635903207598</v>
       </c>
       <c r="B89">
-        <v>6.5000000000000002E-2</v>
+        <v>-0.39862595419847302</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>2.5379999999999998</v>
+        <v>2.4817107484524401</v>
       </c>
       <c r="B90">
-        <v>0.125</v>
+        <v>-0.29694656488549598</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>2.5710000000000002</v>
+        <v>2.4985931344963399</v>
       </c>
       <c r="B91">
-        <v>0.19600000000000001</v>
+        <v>-0.21450381679389299</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>2.6139999999999999</v>
+        <v>2.5098480585255998</v>
       </c>
       <c r="B92">
-        <v>0.29299999999999998</v>
+        <v>-0.15129770992366401</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>2.63</v>
+        <v>2.5154755205402299</v>
       </c>
       <c r="B93">
-        <v>0.36199999999999999</v>
+        <v>-4.1374045801526697E-2</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>2.6520000000000001</v>
+        <v>2.53235790658412</v>
       </c>
       <c r="B94">
-        <v>0.39900000000000002</v>
+        <v>3.2824427480915901E-2</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>2.6960000000000002</v>
+        <v>2.5492402926280202</v>
       </c>
       <c r="B95">
-        <v>0.33</v>
+        <v>6.85496183206106E-2</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>2.734</v>
+        <v>2.5604952166572801</v>
       </c>
       <c r="B96">
-        <v>0.26800000000000002</v>
+        <v>0.112519083969465</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>2.7770000000000001</v>
+        <v>2.5717501406865502</v>
       </c>
       <c r="B97">
-        <v>0.20200000000000001</v>
+        <v>0.14824427480916</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>2.8319999999999999</v>
+        <v>2.5886325267304402</v>
       </c>
       <c r="B98">
-        <v>0.17899999999999999</v>
+        <v>0.19221374045801501</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>2.859</v>
+        <v>2.62239729881823</v>
       </c>
       <c r="B99">
-        <v>0.156</v>
+        <v>0.27190839694656399</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>2.875</v>
+        <v>2.6449071468767502</v>
       </c>
       <c r="B100">
-        <v>0.11</v>
+        <v>0.32412213740458001</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>2.88</v>
+        <v>2.6505346088913799</v>
       </c>
       <c r="B101">
-        <v>2.7E-2</v>
+        <v>0.34610687022900699</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>2.9020000000000001</v>
+        <v>2.67867191896454</v>
       </c>
       <c r="B102">
-        <v>-1.2999999999999999E-2</v>
+        <v>0.387328244274809</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>2.9239999999999999</v>
+        <v>2.6955543050084398</v>
       </c>
       <c r="B103">
-        <v>-6.4000000000000001E-2</v>
+        <v>0.36534351145038102</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>2.9350000000000001</v>
+        <v>2.7293190770962199</v>
       </c>
       <c r="B104">
-        <v>-0.113</v>
+        <v>0.313129770992366</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>2.9510000000000001</v>
+        <v>2.7687113111986399</v>
       </c>
       <c r="B105">
-        <v>-0.15</v>
+        <v>0.22793893129770901</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>2.9620000000000002</v>
+        <v>2.7855936972425401</v>
       </c>
       <c r="B106">
-        <v>-0.22700000000000001</v>
+        <v>0.19221374045801501</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>3.0649999999999999</v>
+        <v>2.8081035453010599</v>
       </c>
       <c r="B107">
-        <v>-0.27</v>
+        <v>0.18122137404580099</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>3.109</v>
+        <v>2.8474957794034799</v>
       </c>
       <c r="B108">
-        <v>-0.19600000000000001</v>
+        <v>0.17572519083969401</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>3.141</v>
+        <v>2.87563308947664</v>
       </c>
       <c r="B109">
-        <v>-0.153</v>
+        <v>0.16473282442748</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>3.1579999999999999</v>
+        <v>2.8868880135058999</v>
       </c>
       <c r="B110">
-        <v>-0.10199999999999999</v>
+        <v>0.131755725190839</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>3.1850000000000001</v>
+        <v>2.8925154755205398</v>
       </c>
       <c r="B111">
-        <v>-0.13600000000000001</v>
+        <v>5.7557251908396903E-2</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>3.2120000000000002</v>
+        <v>2.9375351716375899</v>
       </c>
       <c r="B112">
-        <v>-0.17</v>
+        <v>-4.6870229007633601E-2</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>3.2450000000000001</v>
+        <v>2.9487900956668498</v>
       </c>
       <c r="B113">
-        <v>-0.19600000000000001</v>
+        <v>-0.118320610687022</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>3.2829999999999999</v>
+        <v>2.9769274057400099</v>
       </c>
       <c r="B114">
-        <v>-0.125</v>
+        <v>-0.203511450381679</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>3.3210000000000002</v>
+        <v>2.9825548677546401</v>
       </c>
       <c r="B115">
-        <v>-3.3000000000000002E-2</v>
+        <v>-0.22549618320610601</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>3.37</v>
+        <v>2.9994372537985301</v>
       </c>
       <c r="B116">
-        <v>0.01</v>
+        <v>-0.24748091603053399</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>3.4079999999999999</v>
+        <v>3.0275745638716902</v>
       </c>
       <c r="B117">
-        <v>8.9999999999999993E-3</v>
+        <v>-0.26946564885496099</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>3.4569999999999999</v>
+        <v>3.06133933595948</v>
       </c>
       <c r="B118">
-        <v>-2.8000000000000001E-2</v>
+        <v>-0.28870229007633502</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119">
-        <v>3.5110000000000001</v>
+        <v>3.0951041080472699</v>
       </c>
       <c r="B119">
-        <v>-5.3999999999999999E-2</v>
+        <v>-0.25847328244274798</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>3.516</v>
+        <v>3.1176139561057901</v>
       </c>
       <c r="B120">
-        <v>-2.1999999999999999E-2</v>
+        <v>-0.22274809160305301</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121">
-        <v>3.5379999999999998</v>
+        <v>3.1288688801350499</v>
       </c>
       <c r="B121">
-        <v>3.2000000000000001E-2</v>
+        <v>-0.181526717557251</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>3.62</v>
+        <v>3.14012380416432</v>
       </c>
       <c r="B122">
-        <v>8.3000000000000004E-2</v>
+        <v>-0.14854961832061001</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123">
-        <v>3.6579999999999999</v>
+        <v>3.1626336522228402</v>
       </c>
       <c r="B123">
-        <v>8.1000000000000003E-2</v>
+        <v>-9.6335877862595301E-2</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124">
-        <v>3.7120000000000002</v>
+        <v>3.1851435002813702</v>
       </c>
       <c r="B124">
-        <v>8.3000000000000004E-2</v>
+        <v>-0.126564885496183</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125">
-        <v>3.7549999999999999</v>
+        <v>3.21890827236916</v>
       </c>
       <c r="B125">
-        <v>0.08</v>
+        <v>-0.165038167938931</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126">
-        <v>3.7770000000000001</v>
+        <v>3.2639279684862101</v>
       </c>
       <c r="B126">
-        <v>4.5999999999999999E-2</v>
+        <v>-0.21175572519083899</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127">
-        <v>3.8210000000000002</v>
+        <v>3.29206527855936</v>
       </c>
       <c r="B127">
-        <v>-1.0999999999999999E-2</v>
+        <v>-0.162290076335877</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128">
-        <v>3.8639999999999999</v>
+        <v>3.297692740574</v>
       </c>
       <c r="B128">
-        <v>-3.1E-2</v>
+        <v>-0.126564885496183</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129">
-        <v>3.891</v>
+        <v>3.3483398987056798</v>
       </c>
       <c r="B129">
-        <v>6.0000000000000001E-3</v>
+        <v>-4.9618320610687001E-2</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130">
-        <v>3.9510000000000001</v>
+        <v>3.3821046707934701</v>
       </c>
       <c r="B130">
-        <v>2.3E-2</v>
+        <v>2.59541984732825E-3</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131">
-        <v>3.9950000000000001</v>
+        <v>3.41024198086662</v>
       </c>
       <c r="B131">
-        <v>0</v>
+        <v>1.3587786259541899E-2</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132">
-        <v>4.016</v>
+        <v>3.4552616769836701</v>
       </c>
       <c r="B132">
-        <v>-3.4000000000000002E-2</v>
+        <v>-2.76335877862595E-2</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133">
-        <v>4.0759999999999996</v>
+        <v>3.5115362971299899</v>
       </c>
       <c r="B133">
-        <v>-6.6000000000000003E-2</v>
+        <v>-6.3358778625954099E-2</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134">
-        <v>4.1520000000000001</v>
+        <v>3.5396736072031501</v>
       </c>
       <c r="B134">
-        <v>-5.3999999999999999E-2</v>
+        <v>-1.9389312977099199E-2</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135">
-        <v>4.234</v>
+        <v>3.5565559932470401</v>
       </c>
       <c r="B135">
-        <v>-5.1999999999999998E-2</v>
+        <v>5.3435114503816898E-3</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136">
-        <v>4.2549999999999999</v>
+        <v>3.5621834552616698</v>
       </c>
       <c r="B136">
-        <v>-3.2000000000000001E-2</v>
+        <v>2.4580152671755701E-2</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137">
-        <v>4.2930000000000001</v>
+        <v>3.61845807540799</v>
       </c>
       <c r="B137">
-        <v>-5.8000000000000003E-2</v>
+        <v>6.0305343511450303E-2</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138">
-        <v>4.3319999999999999</v>
+        <v>3.6634777715250402</v>
       </c>
       <c r="B138">
-        <v>-4.5999999999999999E-2</v>
+        <v>8.2290076335877801E-2</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139">
-        <v>4.37</v>
+        <v>3.6972425436128198</v>
       </c>
       <c r="B139">
-        <v>-1.4999999999999999E-2</v>
+        <v>6.5801526717557193E-2</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140">
-        <v>4.4290000000000003</v>
+        <v>3.75351716375914</v>
       </c>
       <c r="B140">
-        <v>1.7000000000000001E-2</v>
+        <v>7.1297709923663993E-2</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141">
-        <v>4.4619999999999997</v>
+        <v>3.79290939786156</v>
       </c>
       <c r="B141">
-        <v>2.1999999999999999E-2</v>
+        <v>2.4580152671755701E-2</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142">
-        <v>4.5330000000000004</v>
+        <v>3.8154192459200802</v>
       </c>
       <c r="B142">
-        <v>1.0999999999999999E-2</v>
+        <v>-8.39694656488554E-3</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143">
-        <v>4.62</v>
+        <v>3.83230163196398</v>
       </c>
       <c r="B143">
-        <v>-1E-3</v>
+        <v>-3.31297709923664E-2</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144">
-        <v>4.6470000000000002</v>
+        <v>3.8660664040517698</v>
       </c>
       <c r="B144">
-        <v>-2.7E-2</v>
+        <v>-4.9618320610687001E-2</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145">
-        <v>4.6790000000000003</v>
+        <v>3.8942037141249202</v>
       </c>
       <c r="B145">
-        <v>-3.2000000000000001E-2</v>
+        <v>-1.6641221374045698E-2</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146">
-        <v>4.7229999999999999</v>
+        <v>3.9223410241980798</v>
       </c>
       <c r="B146">
-        <v>0.01</v>
+        <v>-1.52671755725197E-4</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147">
-        <v>4.7549999999999999</v>
+        <v>3.9448508722566098</v>
       </c>
       <c r="B147">
-        <v>5.2999999999999999E-2</v>
+        <v>5.3435114503816898E-3</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148">
-        <v>4.859</v>
+        <v>3.9842431063590298</v>
       </c>
       <c r="B148">
-        <v>8.6999999999999994E-2</v>
+        <v>-8.39694656488554E-3</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149">
-        <v>4.8860000000000001</v>
+        <v>4.00675295441755</v>
       </c>
       <c r="B149">
-        <v>6.2E-2</v>
+        <v>-3.0381679389313E-2</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150">
-        <v>4.9080000000000004</v>
+        <v>4.0180078784468201</v>
       </c>
       <c r="B150">
-        <v>3.3000000000000002E-2</v>
+        <v>-5.2366412213740499E-2</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151">
-        <v>4.9290000000000003</v>
+        <v>4.0461451885199704</v>
       </c>
       <c r="B151">
-        <v>-4.0000000000000001E-3</v>
+        <v>-7.4351145038167907E-2</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152">
-        <v>4.9669999999999996</v>
+        <v>4.1080472706809203</v>
       </c>
       <c r="B152">
-        <v>-4.3999999999999997E-2</v>
+        <v>-6.3358778625954099E-2</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153">
-        <v>4.9950000000000001</v>
+        <v>4.1418120427687102</v>
       </c>
       <c r="B153">
-        <v>-7.0000000000000001E-3</v>
+        <v>-6.0610687022900699E-2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>4.1812042768711297</v>
+      </c>
+      <c r="B154">
+        <v>-7.4351145038167907E-2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <v>4.2205965109735502</v>
+      </c>
+      <c r="B155">
+        <v>-6.3358778625954099E-2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <v>4.2374788970174402</v>
+      </c>
+      <c r="B156">
+        <v>-4.4122137404580097E-2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <v>4.2599887450759697</v>
+      </c>
+      <c r="B157">
+        <v>-6.0610687022900699E-2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A158">
+        <v>4.2824985931344903</v>
+      </c>
+      <c r="B158">
+        <v>-7.70992366412213E-2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A159">
+        <v>4.3444006752954403</v>
+      </c>
+      <c r="B159">
+        <v>-4.4122137404580097E-2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A160">
+        <v>4.3950478334271201</v>
+      </c>
+      <c r="B160">
+        <v>-1.38931297709923E-2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A161">
+        <v>4.4400675295441703</v>
+      </c>
+      <c r="B161">
+        <v>1.3587786259541899E-2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A162">
+        <v>4.5357343837929003</v>
+      </c>
+      <c r="B162">
+        <v>-1.9389312977099199E-2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A163">
+        <v>4.5751266178953198</v>
+      </c>
+      <c r="B163">
+        <v>-1.9389312977099199E-2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A164">
+        <v>4.6370287000562698</v>
+      </c>
+      <c r="B164">
+        <v>-5.2366412213740499E-2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165">
+        <v>4.7326955543049998</v>
+      </c>
+      <c r="B165">
+        <v>2.4580152671755701E-2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A166">
+        <v>4.8002250984805803</v>
+      </c>
+      <c r="B166">
+        <v>6.5801526717557193E-2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A167">
+        <v>4.8283624085537404</v>
+      </c>
+      <c r="B167">
+        <v>7.6793893129770904E-2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A168">
+        <v>4.8564997186268899</v>
+      </c>
+      <c r="B168">
+        <v>5.7557251908396903E-2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A169">
+        <v>4.8733821046707897</v>
+      </c>
+      <c r="B169">
+        <v>3.0076335877862601E-2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A170">
+        <v>4.90151941474394</v>
+      </c>
+      <c r="B170">
+        <v>-1.9389312977099199E-2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A171">
+        <v>4.9409116488463596</v>
+      </c>
+      <c r="B171">
+        <v>-7.16030534351145E-2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A172">
+        <v>4.9690489589195197</v>
+      </c>
+      <c r="B172">
+        <v>-3.31297709923664E-2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A173">
+        <v>4.9971862689926798</v>
+      </c>
+      <c r="B173">
+        <v>1.3587786259541899E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update data for dummy earthquake
</commit_message>
<xml_diff>
--- a/pynewmarkdisp/earthquake_data_simple.xlsx
+++ b/pynewmarkdisp/earthquake_data_simple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EAMA\My Drive\Dev\GitHub\data4testing\pynewmarkdisp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4AAC8B25-C4C9-4831-AC74-8D2F51624E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8B1C613-CC78-46EF-9738-12AEB82E4C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
@@ -509,9 +509,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -869,7 +868,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B173"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -886,1375 +887,1375 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-2.8571428571432201E-3</v>
+        <v>-2.7905242047618901E-3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2.8137310073157E-2</v>
+        <v>2.8102845290401499E-2</v>
       </c>
       <c r="B3">
-        <v>2.8571428571424399E-3</v>
+        <v>2.9397081099115001E-3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>5.6274620146314E-2</v>
+        <v>5.6140259043456299E-2</v>
       </c>
       <c r="B4">
-        <v>1.1428571428571E-2</v>
+        <v>1.14604646293462E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>7.87844682048396E-2</v>
+        <v>7.8714139428062893E-2</v>
       </c>
       <c r="B5">
-        <v>5.71428571428533E-3</v>
+        <v>5.9987633439437804E-3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>0.10129431626336501</v>
+        <v>0.101353451350016</v>
       </c>
       <c r="B6">
-        <v>-5.7142857142861098E-3</v>
+        <v>-5.0439863509816798E-3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>0.112549240292628</v>
+        <v>0.112738538848339</v>
       </c>
       <c r="B7">
-        <v>-1.71428571428574E-2</v>
+        <v>-1.6146409607967298E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>0.146314012380416</v>
+        <v>0.146762938268616</v>
       </c>
       <c r="B8">
-        <v>-4.0000000000000202E-2</v>
+        <v>-3.8291582559878301E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>0.18570624648283601</v>
+        <v>0.18602186067662699</v>
       </c>
       <c r="B9">
-        <v>-2.85714285714289E-2</v>
+        <v>-2.6920628273621901E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>0.225098480585256</v>
+        <v>0.22537893039065901</v>
       </c>
       <c r="B10">
-        <v>-2.5714285714285998E-2</v>
+        <v>-2.39212466016498E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>0.25323579065841201</v>
+        <v>0.25361263875575302</v>
       </c>
       <c r="B11">
-        <v>-3.4285714285714503E-2</v>
+        <v>-3.2143635310783701E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>0.28137310073156901</v>
+        <v>0.281911778658195</v>
       </c>
       <c r="B12">
-        <v>-4.85714285714288E-2</v>
+        <v>-4.5947072429440503E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>0.34890264490714601</v>
+        <v>0.349437125199975</v>
       </c>
       <c r="B13">
-        <v>-4.85714285714288E-2</v>
+        <v>-4.5589031057079399E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>0.37703995498030302</v>
+        <v>0.377638117796396</v>
       </c>
       <c r="B14">
-        <v>-5.4285714285714402E-2</v>
+        <v>-5.1020895561451798E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>0.40517726505346002</v>
+        <v>0.40587182616149098</v>
       </c>
       <c r="B15">
-        <v>-6.2857142857143E-2</v>
+        <v>-5.9243284270585797E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>0.416432189082723</v>
+        <v>0.417093334816448</v>
       </c>
       <c r="B16">
-        <v>-6.0000000000000199E-2</v>
+        <v>-5.6393086503764102E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>0.450196961170512</v>
+        <v>0.450496134631931</v>
       </c>
       <c r="B17">
-        <v>-2.85714285714289E-2</v>
+        <v>-2.5518299565207701E-2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>0.46145188519977398</v>
+        <v>0.46152134867484701</v>
       </c>
       <c r="B18">
-        <v>-8.5714285714288893E-3</v>
+        <v>-5.9249565698174999E-3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>0.50084411930219397</v>
+        <v>0.50058397647081898</v>
       </c>
       <c r="B19">
-        <v>1.9999999999999501E-2</v>
+        <v>2.2189142945007598E-2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>0.517726505346088</v>
-      </c>
-      <c r="B20" s="1">
-        <v>-3.3306690738754598E-16</v>
+        <v>0.51769432348697697</v>
+      </c>
+      <c r="B20">
+        <v>2.74498385476773E-3</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>0.56274620146314003</v>
+        <v>0.56320195771159698</v>
       </c>
       <c r="B21">
-        <v>-4.28571428571431E-2</v>
+        <v>-3.8874184968413203E-2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>0.57962858750703405</v>
+        <v>0.57978885242898204</v>
       </c>
       <c r="B22">
-        <v>-1.71428571428574E-2</v>
+        <v>-1.36699567824699E-2</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>0.60776589758019095</v>
+        <v>0.607531824263977</v>
       </c>
       <c r="B23">
-        <v>1.7142857142856599E-2</v>
+        <v>1.9965517579817699E-2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>0.65841305571187303</v>
+        <v>0.65850299185704497</v>
       </c>
       <c r="B24">
-        <v>-1.14285714285716E-2</v>
+        <v>-7.6711934385258404E-3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>0.66966797974113601</v>
-      </c>
-      <c r="B25" s="1">
-        <v>-3.3306690738754598E-16</v>
+        <v>0.66962635320598096</v>
+      </c>
+      <c r="B25">
+        <v>3.5505769425800901E-3</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>0.67529544175576794</v>
+        <v>0.67499173926840905</v>
       </c>
       <c r="B26">
-        <v>2.2857142857142399E-2</v>
+        <v>2.5904607361701699E-2</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>0.68092290377039899</v>
+        <v>0.68035712533083803</v>
       </c>
       <c r="B27">
-        <v>4.5714285714285201E-2</v>
+        <v>4.8258637780823399E-2</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>0.69217782779966197</v>
+        <v>0.69134962360508101</v>
       </c>
       <c r="B28">
-        <v>6.8571428571428006E-2</v>
+        <v>7.0642504980975102E-2</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>0.70343275182892495</v>
+        <v>0.70230940611065096</v>
       </c>
       <c r="B29">
-        <v>9.4285714285713695E-2</v>
+        <v>9.5816896385888403E-2</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>0.72031513787281898</v>
+        <v>0.71945246889548198</v>
       </c>
       <c r="B30">
-        <v>7.1428571428570897E-2</v>
+        <v>7.3582213090887E-2</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>0.74845244794597598</v>
+        <v>0.74807876648465799</v>
       </c>
       <c r="B31">
-        <v>2.8571428571428099E-2</v>
+        <v>3.1873533924615803E-2</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>0.77096229600450095</v>
-      </c>
-      <c r="B32" s="1">
-        <v>-3.3306690738754598E-16</v>
+        <v>0.77091437301865096</v>
+      </c>
+      <c r="B32">
+        <v>4.0876390011217404E-3</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>0.79909960607765795</v>
+        <v>0.79878820792833904</v>
       </c>
       <c r="B33">
-        <v>2.2857142857142399E-2</v>
+        <v>2.65610165443637E-2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>0.83849184018007805</v>
+        <v>0.83775268841828998</v>
       </c>
       <c r="B34">
-        <v>5.9999999999999401E-2</v>
+        <v>6.30466886734731E-2</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>0.85537422622397197</v>
+        <v>0.85447044621036805</v>
       </c>
       <c r="B35">
-        <v>7.4285714285713705E-2</v>
+        <v>7.7088820040370598E-2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>0.91727630838491803</v>
+        <v>0.91689213283910698</v>
       </c>
       <c r="B36">
-        <v>2.8571428571428099E-2</v>
+        <v>3.2768637355518403E-2</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>0.95666854248733801</v>
+        <v>0.95608562370977102</v>
       </c>
       <c r="B37">
-        <v>4.5714285714285201E-2</v>
+        <v>4.9720640051297699E-2</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>0.9679234665166</v>
+        <v>0.96776515312615496</v>
       </c>
       <c r="B38">
-        <v>8.5714285714282301E-3</v>
+        <v>1.35034989514591E-2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>0.99043331457512596</v>
+        <v>0.990797054272188</v>
       </c>
       <c r="B39">
-        <v>-3.7142857142857401E-2</v>
+        <v>-3.10255412006036E-2</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>1.01294316263365</v>
+        <v>1.01376352388087</v>
       </c>
       <c r="B40">
-        <v>-7.7142857142857194E-2</v>
+        <v>-6.9973532943143402E-2</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>1.03545301069217</v>
+        <v>1.0360429623474201</v>
       </c>
       <c r="B41">
-        <v>-5.7142857142857301E-2</v>
+        <v>-5.0320516385693001E-2</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>1.0410804727067999</v>
+        <v>1.0414410641785199</v>
       </c>
       <c r="B42">
-        <v>-3.7142857142857401E-2</v>
+        <v>-3.07570101713328E-2</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>1.06921778277996</v>
+        <v>1.0690858887074901</v>
       </c>
       <c r="B43">
-        <v>5.71428571428533E-3</v>
+        <v>1.12500368052392E-2</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>1.1029825548677501</v>
+        <v>1.1034047300458301</v>
       </c>
       <c r="B44">
-        <v>-4.28571428571431E-2</v>
+        <v>-3.60098539895247E-2</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>1.11423747889701</v>
+        <v>1.1149206806188501</v>
       </c>
       <c r="B45">
-        <v>-6.5714285714285794E-2</v>
+        <v>-5.8274374065556099E-2</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>1.1254924029262701</v>
+        <v>1.1263384838858399</v>
       </c>
       <c r="B46">
-        <v>-8.0000000000000099E-2</v>
+        <v>-7.2167321527303194E-2</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>1.15362971299943</v>
+        <v>1.1548666341689999</v>
       </c>
       <c r="B47">
-        <v>-0.114285714285714</v>
+        <v>-0.10550442807929</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>1.1817670230725901</v>
+        <v>1.1828059006160301</v>
       </c>
       <c r="B48">
-        <v>-9.7142857142857197E-2</v>
+        <v>-8.86120989455709E-2</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>1.2211592571750101</v>
+        <v>1.2219666757180201</v>
       </c>
       <c r="B49">
-        <v>-7.7142857142857194E-2</v>
+        <v>-6.8869572045030095E-2</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>1.24929656724817</v>
+        <v>1.25036396292649</v>
       </c>
       <c r="B50">
-        <v>-0.1</v>
+        <v>-9.1044581777971298E-2</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>1.26617895329206</v>
+        <v>1.2673434468679501</v>
       </c>
       <c r="B51">
-        <v>-0.108571428571428</v>
+        <v>-9.93266440491654E-2</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>1.2886888013505899</v>
+        <v>1.28952473802848</v>
       </c>
       <c r="B52">
-        <v>-8.0000000000000099E-2</v>
+        <v>-7.1302054877430507E-2</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>1.3111986494091099</v>
+        <v>1.3116078818829799</v>
       </c>
       <c r="B53">
-        <v>-4.28571428571431E-2</v>
+        <v>-3.49058930914114E-2</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>1.3562183455261601</v>
+        <v>1.3569192214955601</v>
       </c>
       <c r="B54">
-        <v>-6.85714285714287E-2</v>
+        <v>-5.9781916686023701E-2</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>1.3899831176139501</v>
+        <v>1.39045288438574</v>
       </c>
       <c r="B55">
-        <v>-4.85714285714288E-2</v>
+        <v>-4.00692265665131E-2</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>1.4124929656724801</v>
+        <v>1.41276503862096</v>
       </c>
       <c r="B56">
-        <v>-3.1428571428571597E-2</v>
+        <v>-2.32067342138241E-2</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>1.45751266178953</v>
+        <v>1.45781465208415</v>
       </c>
       <c r="B57">
-        <v>-3.4285714285714503E-2</v>
+        <v>-2.5758564170344798E-2</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>1.4856499718626801</v>
-      </c>
-      <c r="B58" s="1">
-        <v>-3.3306690738754598E-16</v>
+        <v>1.4855576239191499</v>
+      </c>
+      <c r="B58">
+        <v>7.87691019194303E-3</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>1.5250422059651001</v>
+        <v>1.5240967994163499</v>
       </c>
       <c r="B59">
-        <v>7.4285714285713705E-2</v>
+        <v>8.0639396982951195E-2</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>1.57006190208216</v>
+        <v>1.5699970228650499</v>
       </c>
       <c r="B60">
-        <v>-2.8571428571432201E-3</v>
+        <v>5.5339377026328799E-3</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>1.59257175014068</v>
+        <v>1.5930616397797499</v>
       </c>
       <c r="B61">
-        <v>-5.1428571428571601E-2</v>
+        <v>-4.1785626654191298E-2</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>1.6769836803601501</v>
+        <v>1.67818806986779</v>
       </c>
       <c r="B62">
-        <v>-0.114285714285714</v>
+        <v>-0.10272960744349099</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>1.78390545863815</v>
+        <v>1.7852667807356399</v>
       </c>
       <c r="B63">
-        <v>-0.128571428571428</v>
+        <v>-0.116115329627727</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>1.82329769274057</v>
+        <v>1.82439484006896</v>
       </c>
       <c r="B64">
-        <v>-0.105714285714285</v>
+        <v>-9.3582278522424997E-2</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>1.87394485087225</v>
+        <v>1.8753332918933501</v>
       </c>
       <c r="B65">
-        <v>-0.13142857142857101</v>
+        <v>-0.118428465336007</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>1.9245920090039299</v>
+        <v>1.9258137229563199</v>
       </c>
       <c r="B66">
-        <v>-0.11714285714285699</v>
+        <v>-0.104207313282929</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>1.97523916713562</v>
+        <v>1.9766540274747</v>
       </c>
       <c r="B67">
-        <v>-0.13428571428571401</v>
+        <v>-0.120681927482227</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>2.00900393922341</v>
+        <v>2.0095660907600799</v>
       </c>
       <c r="B68">
-        <v>-6.0000000000000199E-2</v>
+        <v>-4.7949277472249197E-2</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>2.0371412492965599</v>
+        <v>2.03688375760232</v>
       </c>
       <c r="B69">
-        <v>1.1428571428571E-2</v>
+        <v>2.19630115519374E-2</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>2.0596510973550899</v>
+        <v>2.0590650487628501</v>
       </c>
       <c r="B70">
-        <v>3.9999999999999397E-2</v>
+        <v>4.9987600723672199E-2</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>2.0877884074282398</v>
+        <v>2.0862845682990701</v>
       </c>
       <c r="B71">
-        <v>0.119999999999999</v>
+        <v>0.12827146236214301</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>2.1102982554867702</v>
+        <v>2.1079424071608202</v>
       </c>
       <c r="B72">
-        <v>0.19428571428571301</v>
+        <v>0.20094443881006099</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>2.14406302757456</v>
+        <v>2.1410671229425802</v>
       </c>
       <c r="B73">
-        <v>0.249999999999998</v>
+        <v>0.25553868148908898</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>2.14687675858187</v>
+        <v>2.14337358463405</v>
       </c>
       <c r="B74">
-        <v>0.29428571428571199</v>
+        <v>0.298806725053407</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>2.1722003376477201</v>
+        <v>2.1682702845944699</v>
       </c>
       <c r="B75">
-        <v>0.33142857142857002</v>
+        <v>0.33521780522994099</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>2.18345526167698</v>
+        <v>2.1790664882566699</v>
       </c>
       <c r="B76">
-        <v>0.37142857142857</v>
+        <v>0.37434481765866101</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>2.1975239167135601</v>
+        <v>2.1925781007187601</v>
       </c>
       <c r="B77">
-        <v>0.41999999999999799</v>
+        <v>0.42185832109218102</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>2.2341024198086599</v>
+        <v>2.2284345831847401</v>
       </c>
       <c r="B78">
-        <v>0.48285714285714099</v>
+        <v>0.48344379267362902</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>2.2734946539110799</v>
+        <v>2.2685441155782602</v>
       </c>
       <c r="B79">
-        <v>0.41999999999999799</v>
+        <v>0.42226111763608698</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>2.2734946539110799</v>
+        <v>2.26896942057102</v>
       </c>
       <c r="B80">
-        <v>0.38285714285714101</v>
+        <v>0.38598430297418901</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>2.2960045019696098</v>
+        <v>2.2926556370905198</v>
       </c>
       <c r="B81">
-        <v>0.27999999999999797</v>
+        <v>0.28564477872689698</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>2.30163196398424</v>
+        <v>2.2992642223625301</v>
       </c>
       <c r="B82">
-        <v>0.19428571428571301</v>
+        <v>0.20195888936508399</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>2.3128868880134998</v>
+        <v>2.3098504998424101</v>
       </c>
       <c r="B83">
-        <v>6.5714285714285101E-2</v>
+        <v>5.8991765441024399E-2</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>2.3353967360720298</v>
+        <v>2.3353824309779001</v>
       </c>
       <c r="B84">
-        <v>-1.14285714285716E-2</v>
+        <v>1.2201673084405399E-3</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>2.3691615081598201</v>
+        <v>2.3706827453764401</v>
       </c>
       <c r="B85">
-        <v>-0.14571428571428499</v>
+        <v>-0.12975544962916599</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>2.3916713562183398</v>
+        <v>2.3943689618959398</v>
       </c>
       <c r="B86">
-        <v>-0.248571428571428</v>
+        <v>-0.230094973876458</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>2.39729881823297</v>
+        <v>2.4005849579438698</v>
       </c>
       <c r="B87">
-        <v>-0.29999999999999899</v>
+        <v>-0.28029457278113401</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>2.4029262802476001</v>
+        <v>2.40699724860385</v>
       </c>
       <c r="B88">
-        <v>-0.36857142857142799</v>
+        <v>-0.34723731691437898</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>2.4310635903207598</v>
+        <v>2.43572169349904</v>
       </c>
       <c r="B89">
-        <v>-0.41999999999999899</v>
+        <v>-0.39731756869493401</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>2.4817107484524401</v>
+        <v>2.48515521996447</v>
       </c>
       <c r="B90">
-        <v>-0.314285714285713</v>
+        <v>-0.29379964208949</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>2.4985931344963399</v>
+        <v>2.5010550835397098</v>
       </c>
       <c r="B91">
-        <v>-0.22857142857142801</v>
+        <v>-0.20999440560355601</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>2.5098480585255998</v>
+        <v>2.5115568452838501</v>
       </c>
       <c r="B92">
-        <v>-0.16285714285714201</v>
+        <v>-0.14575267533198299</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>2.5154755205402299</v>
+        <v>2.5158753267487302</v>
       </c>
       <c r="B93">
-        <v>-4.85714285714288E-2</v>
+        <v>-3.41018703604953E-2</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>2.53235790658412</v>
+        <v>2.53187333763</v>
       </c>
       <c r="B94">
-        <v>2.8571428571428099E-2</v>
+        <v>4.1331793511153903E-2</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>2.5492402926280202</v>
+        <v>2.54832936927269</v>
       </c>
       <c r="B95">
-        <v>6.5714285714285101E-2</v>
+        <v>7.7698118516143E-2</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>2.5604952166572801</v>
+        <v>2.5590601413975498</v>
       </c>
       <c r="B96">
-        <v>0.11142857142857</v>
+        <v>0.122406179354386</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>2.5717501406865502</v>
+        <v>2.5698890608284199</v>
       </c>
       <c r="B97">
-        <v>0.14857142857142699</v>
+        <v>0.15874266757834499</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>2.5886325267304402</v>
+        <v>2.5862469451651</v>
       </c>
       <c r="B98">
-        <v>0.19428571428571301</v>
+        <v>0.20348056519761801</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>2.62239729881823</v>
+        <v>2.6167162310562002</v>
       </c>
       <c r="B99">
-        <v>0.27714285714285603</v>
+        <v>0.28457235582978502</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>2.6449071468767502</v>
+        <v>2.6386030802986702</v>
       </c>
       <c r="B100">
-        <v>0.33142857142857002</v>
+        <v>0.33771166284437298</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>2.6505346088913799</v>
+        <v>2.64631309644935</v>
       </c>
       <c r="B101">
-        <v>0.35428571428571298</v>
+        <v>0.36007812525559002</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>2.67867191896454</v>
+        <v>2.6738216052755202</v>
       </c>
       <c r="B102">
-        <v>0.40428571428571197</v>
+        <v>0.41371235641866799</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>2.6955543050084398</v>
+        <v>2.6911009837631599</v>
       </c>
       <c r="B103">
-        <v>0.374285714285712</v>
+        <v>0.379850488937161</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>2.7265053460889099</v>
+        <v>2.7225735532269102</v>
       </c>
       <c r="B104">
-        <v>0.32857142857142702</v>
+        <v>0.33536620395664302</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>2.7687113111986399</v>
+        <v>2.7658892309504202</v>
       </c>
       <c r="B105">
-        <v>0.23142857142857001</v>
+        <v>0.24071215685248001</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>2.7855936972425401</v>
+        <v>2.7879396590362502</v>
       </c>
       <c r="B106">
-        <v>0.19428571428571301</v>
+        <v>0.19989884284326101</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>2.8081035453010599</v>
+        <v>2.81053807624737</v>
       </c>
       <c r="B107">
-        <v>0.182857142857141</v>
+        <v>0.19234424840428699</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>2.8474957794034799</v>
+        <v>2.8452904015206202</v>
       </c>
       <c r="B108">
-        <v>0.17714285714285599</v>
+        <v>0.188109911896434</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>2.87563308947664</v>
+        <v>2.87355682565439</v>
       </c>
       <c r="B109">
-        <v>0.16571428571428401</v>
+        <v>0.177096998982538</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>2.8868880135058999</v>
+        <v>2.8827226935110399</v>
       </c>
       <c r="B110">
-        <v>0.13142857142857001</v>
+        <v>0.15528513428187099</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>2.8925154755205398</v>
+        <v>2.8917140772680998</v>
       </c>
       <c r="B111">
-        <v>5.4285714285713701E-2</v>
+        <v>6.8356065339932603E-2</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>2.9375351716375899</v>
+        <v>2.9379741741721999</v>
       </c>
       <c r="B112">
-        <v>-5.4285714285714402E-2</v>
+        <v>-3.7445160192761499E-2</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>2.9487900956668498</v>
+        <v>2.9500790085813402</v>
       </c>
       <c r="B113">
-        <v>-0.128571428571428</v>
+        <v>-0.109939115954499</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>2.9769274057400099</v>
+        <v>2.97922875846929</v>
       </c>
       <c r="B114">
-        <v>-0.217142857142856</v>
+        <v>-0.19629618239695301</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>2.9825548677546401</v>
+        <v>2.9851175968304902</v>
       </c>
       <c r="B115">
-        <v>-0.23999999999999899</v>
+        <v>-0.218590539254014</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>2.9994372537985301</v>
+        <v>3.0022606596153198</v>
       </c>
       <c r="B116">
-        <v>-0.26285714285714201</v>
+        <v>-0.240825222549016</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>3.0275745638716902</v>
+        <v>3.03065794682378</v>
       </c>
       <c r="B117">
-        <v>-0.28571428571428498</v>
+        <v>-0.26300023228195701</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>3.06133933595948</v>
+        <v>3.0646496304753899</v>
       </c>
       <c r="B118">
-        <v>-0.30571428571428499</v>
+        <v>-0.282354881029107</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119">
-        <v>3.0951041080472699</v>
+        <v>3.0980524302908701</v>
       </c>
       <c r="B119">
-        <v>-0.27428571428571302</v>
+        <v>-0.25148009409055</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>3.1176139561057901</v>
+        <v>3.12013557414538</v>
       </c>
       <c r="B120">
-        <v>-0.23714285714285599</v>
+        <v>-0.21508393230453099</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121">
-        <v>3.1288688801350499</v>
+        <v>3.1308990620389099</v>
       </c>
       <c r="B121">
-        <v>-0.19428571428571401</v>
+        <v>-0.17316639567104899</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>3.14012380416432</v>
+        <v>3.14176069723846</v>
       </c>
       <c r="B122">
-        <v>-0.159999999999999</v>
+        <v>-0.13962043165185201</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123">
-        <v>3.1626336522228402</v>
+        <v>3.1636475464809202</v>
       </c>
       <c r="B123">
-        <v>-0.105714285714285</v>
+        <v>-8.6481124637263901E-2</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124">
-        <v>3.1851435002813702</v>
+        <v>3.1865158687835899</v>
       </c>
       <c r="B124">
-        <v>-0.13714285714285701</v>
+        <v>-0.117057543765519</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125">
-        <v>3.21890827236916</v>
+        <v>3.2207365628159099</v>
       </c>
       <c r="B125">
-        <v>-0.17714285714285699</v>
+        <v>-0.15594586194599899</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126">
-        <v>3.2639279684862101</v>
+        <v>3.2663505232887098</v>
       </c>
       <c r="B126">
-        <v>-0.22571428571428501</v>
+        <v>-0.20663423443465501</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127">
-        <v>3.29206527855936</v>
+        <v>3.2938563058008299</v>
       </c>
       <c r="B127">
-        <v>-0.17428571428571399</v>
+        <v>-0.15276745958784599</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128">
-        <v>3.297692740574</v>
+        <v>3.2990581130198899</v>
       </c>
       <c r="B128">
-        <v>-0.13714285714285701</v>
+        <v>-0.11646080814491699</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129">
-        <v>3.3483398987056798</v>
+        <v>3.3487860814033699</v>
       </c>
       <c r="B129">
-        <v>-5.7142857142857301E-2</v>
+        <v>-3.8057599382326598E-2</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130">
-        <v>3.3821046707934701</v>
+        <v>3.3819271550694698</v>
       </c>
       <c r="B130">
-        <v>-2.8571428571432201E-3</v>
+        <v>1.51413811943214E-2</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131">
-        <v>3.41024198086662</v>
+        <v>3.40993185305385</v>
       </c>
       <c r="B131">
-        <v>8.5714285714282301E-3</v>
+        <v>2.64526619185175E-2</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132">
-        <v>3.4552616769836701</v>
+        <v>3.4554394872784702</v>
       </c>
       <c r="B132">
-        <v>-3.4285714285714503E-2</v>
+        <v>-1.5166506904663301E-2</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133">
-        <v>3.5115362971299899</v>
+        <v>3.5121359143893698</v>
       </c>
       <c r="B133">
-        <v>-7.1428571428571494E-2</v>
+        <v>-5.1144953756261102E-2</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134">
-        <v>3.5396736072031501</v>
+        <v>3.5397480231496701</v>
       </c>
       <c r="B134">
-        <v>-2.5714285714285998E-2</v>
+        <v>-6.3473825749277204E-3</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135">
-        <v>3.5565559932470401</v>
-      </c>
-      <c r="B135" s="1">
-        <v>-3.3306690738754598E-16</v>
+        <v>3.5563349178670598</v>
+      </c>
+      <c r="B135">
+        <v>1.88568456110156E-2</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136">
-        <v>3.5621834552616698</v>
+        <v>3.5617330196981598</v>
       </c>
       <c r="B136">
-        <v>1.9999999999999501E-2</v>
+        <v>3.8420351825375801E-2</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137">
-        <v>3.61845807540799</v>
+        <v>3.6175788368235602</v>
       </c>
       <c r="B137">
-        <v>5.71428571428566E-2</v>
+        <v>7.4995534297575495E-2</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138">
-        <v>3.6634777715250402</v>
+        <v>3.6623340083686902</v>
       </c>
       <c r="B138">
-        <v>7.9999999999999405E-2</v>
+        <v>9.75584221839077E-2</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139">
-        <v>3.6972425436128198</v>
+        <v>3.6962929762516201</v>
       </c>
       <c r="B139">
-        <v>6.2857142857142306E-2</v>
+        <v>8.0994297641519594E-2</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140">
-        <v>3.75351716375914</v>
+        <v>3.7524986668324201</v>
       </c>
       <c r="B140">
-        <v>6.8571428571428006E-2</v>
+        <v>8.6873713861343294E-2</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141">
-        <v>3.79290939786156</v>
+        <v>3.7924446203825699</v>
       </c>
       <c r="B141">
-        <v>1.9999999999999501E-2</v>
+        <v>3.9643659847609397E-2</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142">
-        <v>3.8154192459200802</v>
+        <v>3.8153456584539098</v>
       </c>
       <c r="B142">
-        <v>-1.42857142857145E-2</v>
+        <v>6.2767165145923799E-3</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143">
-        <v>3.83230163196398</v>
+        <v>3.8325214370074199</v>
       </c>
       <c r="B143">
-        <v>-4.0000000000000202E-2</v>
+        <v>-1.8748490985170198E-2</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144">
-        <v>3.8660664040517698</v>
+        <v>3.8664804048903498</v>
       </c>
       <c r="B144">
-        <v>-5.7142857142857301E-2</v>
+        <v>-3.5312615527558398E-2</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145">
-        <v>3.8942037141249202</v>
+        <v>3.89422337672534</v>
       </c>
       <c r="B145">
-        <v>-2.28571428571431E-2</v>
+        <v>-1.6771411652706199E-3</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146">
-        <v>3.9223410241980798</v>
+        <v>3.9221626431723799</v>
       </c>
       <c r="B146">
-        <v>-5.7142857142861098E-3</v>
+        <v>1.5215187968448399E-2</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147">
-        <v>3.9448508722566098</v>
-      </c>
-      <c r="B147" s="1">
-        <v>-3.3306690738754598E-16</v>
+        <v>3.9446056604822899</v>
+      </c>
+      <c r="B147">
+        <v>2.0915583502091599E-2</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148">
-        <v>3.9842431063590298</v>
+        <v>3.9841590248083598</v>
       </c>
       <c r="B148">
-        <v>-1.42857142857145E-2</v>
+        <v>7.1718199454950896E-3</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149">
-        <v>4.00675295441755</v>
+        <v>4.0069291998050103</v>
       </c>
       <c r="B149">
-        <v>-3.7142857142857401E-2</v>
+        <v>-1.5033026568476099E-2</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150">
-        <v>4.0180078784468201</v>
+        <v>4.0184451503780299</v>
       </c>
       <c r="B150">
-        <v>-6.0000000000000199E-2</v>
+        <v>-3.7297546644507497E-2</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151">
-        <v>4.0461451885199704</v>
+        <v>4.0468424375864904</v>
       </c>
       <c r="B151">
-        <v>-8.2857142857142893E-2</v>
+        <v>-5.9472556377448603E-2</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152">
-        <v>4.1080472706809203</v>
+        <v>4.1086098088417602</v>
       </c>
       <c r="B152">
-        <v>-7.1428571428571494E-2</v>
+        <v>-4.7982254967071702E-2</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153">
-        <v>4.1418120427687102</v>
+        <v>4.14233976634398</v>
       </c>
       <c r="B153">
-        <v>-6.85714285714287E-2</v>
+        <v>-4.5012710076129898E-2</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154">
-        <v>4.1812042768711297</v>
+        <v>4.1818931306700504</v>
       </c>
       <c r="B154">
-        <v>-8.2857142857142893E-2</v>
+        <v>-5.87564736327265E-2</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155">
-        <v>4.2205965109735502</v>
+        <v>4.2211520530780602</v>
       </c>
       <c r="B155">
-        <v>-7.1428571428571494E-2</v>
+        <v>-4.7385519346469999E-2</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156">
-        <v>4.2374788970174402</v>
+        <v>4.2378043793327898</v>
       </c>
       <c r="B156">
-        <v>-5.1428571428571601E-2</v>
+        <v>-2.7762339570049699E-2</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157">
-        <v>4.2599887450759697</v>
+        <v>4.2605091227920902</v>
       </c>
       <c r="B157">
-        <v>-6.85714285714287E-2</v>
+        <v>-4.4386137674497998E-2</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158">
-        <v>4.2824985931344903</v>
+        <v>4.2832138662513897</v>
       </c>
       <c r="B158">
-        <v>-8.5714285714285798E-2</v>
+        <v>-6.1009935778946298E-2</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159">
-        <v>4.3444006752954403</v>
+        <v>4.3447195113572796</v>
       </c>
       <c r="B159">
-        <v>-5.1428571428571601E-2</v>
+        <v>-2.7195440730477999E-2</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160">
-        <v>4.3950478334271201</v>
+        <v>4.3950036478082</v>
       </c>
       <c r="B160">
-        <v>-2.0000000000000202E-2</v>
+        <v>3.7688565511686499E-3</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161">
-        <v>4.4400675295441703</v>
+        <v>4.4396933878159901</v>
       </c>
       <c r="B161">
-        <v>8.5714285714282301E-3</v>
+        <v>3.1912792847023801E-2</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162">
-        <v>4.5357343837929003</v>
+        <v>4.5357468846409201</v>
       </c>
       <c r="B162">
-        <v>-2.5714285714285998E-2</v>
+        <v>-1.06627233260203E-3</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163">
-        <v>4.5751266178953198</v>
+        <v>4.57513667012363</v>
       </c>
       <c r="B163">
-        <v>-2.5714285714285998E-2</v>
+        <v>-8.5741486539137003E-4</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164">
-        <v>4.6370287000562698</v>
+        <v>4.63742749367767</v>
       </c>
       <c r="B164">
-        <v>-6.0000000000000199E-2</v>
+        <v>-3.4015500731197697E-2</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165">
-        <v>4.7326955543049998</v>
+        <v>4.73217235975567</v>
       </c>
       <c r="B165">
-        <v>1.9999999999999501E-2</v>
+        <v>4.46264022796342E-2</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166">
-        <v>4.8002250984805803</v>
+        <v>4.7992069697673498</v>
       </c>
       <c r="B166">
-        <v>6.2857142857142306E-2</v>
+        <v>8.6842306723416904E-2</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167">
-        <v>4.8283624085537404</v>
+        <v>4.8272116677517296</v>
       </c>
       <c r="B167">
-        <v>7.4285714285713705E-2</v>
+        <v>9.8153587447613197E-2</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168">
-        <v>4.8564997186268899</v>
+        <v>4.85557623919152</v>
       </c>
       <c r="B168">
-        <v>5.4285714285713701E-2</v>
+        <v>7.8769101919433496E-2</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169">
-        <v>4.8733821046707897</v>
+        <v>4.8727847335136998</v>
       </c>
       <c r="B169">
-        <v>2.57142857142852E-2</v>
+        <v>5.0953370214909303E-2</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170">
-        <v>4.90151941474394</v>
+        <v>4.9015091784089</v>
       </c>
       <c r="B170">
-        <v>-2.5714285714285998E-2</v>
+        <v>8.7311843435378101E-4</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171">
-        <v>4.9409116488463596</v>
+        <v>4.9415205634964003</v>
       </c>
       <c r="B171">
-        <v>-8.0000000000000099E-2</v>
+        <v>-5.1937983988903098E-2</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172">
-        <v>4.9690489589195197</v>
+        <v>4.9691981037940396</v>
       </c>
       <c r="B172">
-        <v>-4.0000000000000202E-2</v>
+        <v>-1.2721461217092301E-2</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173">
-        <v>4.9971862689926798</v>
+        <v>4.9967774967856702</v>
       </c>
       <c r="B173">
-        <v>8.5714285714282301E-3</v>
+        <v>3.4866634169002597E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>